<commit_message>
Update File Layouts for zip files (#6)
* IBM lab faq and social

* add Start Here

* Update layout of zip files
</commit_message>
<xml_diff>
--- a/PUSH/CallforCodeDayPlan-Worksheet.xlsx
+++ b/PUSH/CallforCodeDayPlan-Worksheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timro/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timro/Desktop/CFC/digital-call-kits/src/PUSH/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F040F105-ED5A-6047-B88E-7811C71E5AC7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7CD0422-12FA-3F49-B78A-604C649F3D81}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="880" windowWidth="27640" windowHeight="16000" xr2:uid="{5A7AAFEF-A55D-B647-B881-725EFD563BC8}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="159">
   <si>
     <t>Ref</t>
   </si>
@@ -494,6 +494,15 @@
   </si>
   <si>
     <t>IBM will be sending you a box of Call for Code swag for distribution during the Call for Code day, but as internal registrations are coming in, consider what other organization items you will want to also provide participants at or shortly after the event. Items can be door prizes or also recognition items to distribute as teams submit their projects to the challenge.</t>
+  </si>
+  <si>
+    <t>Get your Box</t>
+  </si>
+  <si>
+    <t>Send an email to derek.teay@ibm.com with the number of developers that will be attending your Call for Code day and your shipping address</t>
+  </si>
+  <si>
+    <t>C11</t>
   </si>
 </sst>
 </file>
@@ -917,11 +926,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6968080-2ECB-F347-8DA2-0E83BA0038A9}">
-  <dimension ref="A1:AI44"/>
+  <dimension ref="A1:AI45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1176,48 +1185,48 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="5" customFormat="1" ht="97">
+    <row r="17" spans="1:6" s="5" customFormat="1" ht="33">
       <c r="A17" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="5" customFormat="1" ht="49">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="5" customFormat="1" ht="97">
       <c r="A18" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>44</v>
+        <v>153</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="5" customFormat="1" ht="113">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="5" customFormat="1" ht="49">
       <c r="A19" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="5" customFormat="1" ht="97">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="5" customFormat="1" ht="113">
       <c r="A20" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="5" customFormat="1" ht="97">
@@ -1225,271 +1234,282 @@
         <v>55</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="5" customFormat="1" ht="81">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="5" customFormat="1" ht="97">
       <c r="A22" s="5" t="s">
         <v>154</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="5" customFormat="1" ht="81">
+      <c r="A23" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="24">
-      <c r="A23" s="9" t="s">
+    <row r="24" spans="1:6" ht="24">
+      <c r="A24" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="8" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" s="5" customFormat="1" ht="97">
-      <c r="A25" s="5" t="s">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" s="5" customFormat="1" ht="97">
+      <c r="A26" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B26" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="5" customFormat="1" ht="19">
-      <c r="A26" s="5" t="s">
+    <row r="27" spans="1:6" s="5" customFormat="1" ht="19">
+      <c r="A27" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B27" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="5" customFormat="1" ht="49">
-      <c r="A27" s="5" t="s">
+    <row r="28" spans="1:6" s="5" customFormat="1" ht="49">
+      <c r="A28" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B28" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="5" customFormat="1" ht="33">
-      <c r="A28" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="5" customFormat="1" ht="33">
       <c r="A29" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="5" customFormat="1" ht="33">
+      <c r="A30" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="5" customFormat="1" ht="38">
-      <c r="A30" s="5" t="s">
+    <row r="31" spans="1:6" s="5" customFormat="1" ht="38">
+      <c r="A31" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B31" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="5" customFormat="1" ht="33">
-      <c r="A31" s="5" t="s">
+    <row r="32" spans="1:6" s="5" customFormat="1" ht="33">
+      <c r="A32" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B32" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="5" customFormat="1" ht="38">
-      <c r="A32" s="5" t="s">
+    <row r="33" spans="1:3" s="5" customFormat="1" ht="38">
+      <c r="A33" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B33" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="5" customFormat="1" ht="33">
-      <c r="A33" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="5" customFormat="1" ht="33">
       <c r="A34" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="5" customFormat="1" ht="33">
       <c r="A35" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="5" customFormat="1" ht="33">
+      <c r="A36" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B36" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C36" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="5" customFormat="1" ht="49">
-      <c r="A36" s="5" t="s">
+    <row r="37" spans="1:3" s="5" customFormat="1" ht="49">
+      <c r="A37" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B37" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C37" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="5" customFormat="1" ht="81">
-      <c r="A37" s="5" t="s">
+    <row r="38" spans="1:3" s="5" customFormat="1" ht="81">
+      <c r="A38" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B38" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="5" customFormat="1" ht="113">
-      <c r="A38" s="5" t="s">
+    <row r="39" spans="1:3" s="5" customFormat="1" ht="113">
+      <c r="A39" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B39" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="5" customFormat="1" ht="97">
-      <c r="A39" s="5" t="s">
+    <row r="40" spans="1:3" s="5" customFormat="1" ht="97">
+      <c r="A40" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B40" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" s="5" customFormat="1" ht="81">
-      <c r="A40" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:3" s="5" customFormat="1" ht="81">
       <c r="A41" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" s="5" customFormat="1" ht="145">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="5" customFormat="1" ht="81">
       <c r="A42" s="5" t="s">
         <v>108</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="5" customFormat="1" ht="145">
+      <c r="A43" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C43" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="5" customFormat="1" ht="81">
-      <c r="A43" s="5" t="s">
+    <row r="44" spans="1:3" s="5" customFormat="1" ht="81">
+      <c r="A44" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B44" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C44" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="5" customFormat="1" ht="65">
-      <c r="A44" s="5" t="s">
+    <row r="45" spans="1:3" s="5" customFormat="1" ht="65">
+      <c r="A45" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B45" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C45" s="5" t="s">
         <v>118</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A25:F25"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A24:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>